<commit_message>
update usable data sheet
</commit_message>
<xml_diff>
--- a/code/eyeballs_subs_usable_data.xlsx
+++ b/code/eyeballs_subs_usable_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/istart-eyeballs/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F7B7D7-8453-7242-824D-7407D6242F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0427FBF-A94C-B04A-9B44-9216D419711F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14860" yWindow="500" windowWidth="13940" windowHeight="16520" xr2:uid="{8C2BD5BD-9991-FA46-A900-61B8F5B7F454}"/>
+    <workbookView xWindow="14860" yWindow="500" windowWidth="13940" windowHeight="16480" xr2:uid="{8C2BD5BD-9991-FA46-A900-61B8F5B7F454}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -469,9 +469,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E9611E-543E-AB43-AD56-60F2F43FDE89}">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F2" sqref="F2"/>
+      <selection pane="topRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>